<commit_message>
# Conflicts: #	Katana/ProjectSettings/EditorBuildSettings.asset
</commit_message>
<xml_diff>
--- a/仕様書.xlsx
+++ b/仕様書.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="28035" windowHeight="13230"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="28035" windowHeight="13230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
     <sheet name="画面フロー" sheetId="2" r:id="rId2"/>
     <sheet name="影ギミック" sheetId="3" r:id="rId3"/>
     <sheet name="操作方法" sheetId="4" r:id="rId4"/>
+    <sheet name="敵キャラクター" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>影の中でできること</t>
     <rPh sb="0" eb="1">
@@ -222,6 +223,36 @@
     </rPh>
     <rPh sb="29" eb="31">
       <t>ヨテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ネズミ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://blog.livedoor.jp/ebiflynageruyo/archives/38054889.html</t>
+  </si>
+  <si>
+    <t>基本はネズミやふくろうなど, 現実の動物を模したモデル</t>
+    <rPh sb="0" eb="2">
+      <t>キホン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ゲンジツ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ドウブツ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>githubのwiki参照</t>
+    <rPh sb="11" eb="13">
+      <t>サンショウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1048,15 +1079,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>67236</xdr:colOff>
+      <xdr:colOff>212914</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4001</xdr:rowOff>
+      <xdr:rowOff>60030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>434630</xdr:colOff>
+      <xdr:colOff>580308</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>41282</xdr:rowOff>
+      <xdr:rowOff>97311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1079,7 +1110,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="67236" y="2693413"/>
+          <a:off x="212914" y="396206"/>
           <a:ext cx="6519423" cy="4732546"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1173,6 +1204,66 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1" descr="c2260"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="76200" y="1333500"/>
+          <a:ext cx="5448300" cy="2819400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1496,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
@@ -1533,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K3:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1604,11 +1695,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>